<commit_message>
add vco and vca control
</commit_message>
<xml_diff>
--- a/pico-synth-sound/control_stream_format.xlsx
+++ b/pico-synth-sound/control_stream_format.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e6113d96ddfeabfd/22_Development/34_pico_synth/pico-synth-sound/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="823" documentId="11_AD4D066CA252ABDACC10482671D4FCC273EEDF51" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA9DCEFC-9CE7-454F-B1C3-4A1515A22423}"/>
+  <xr:revisionPtr revIDLastSave="826" documentId="11_AD4D066CA252ABDACC10482671D4FCC273EEDF51" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2EEAFA67-C2E8-45F8-A956-2F0147D7C5E7}"/>
   <bookViews>
-    <workbookView xWindow="9135" yWindow="0" windowWidth="19770" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3490,8 +3490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A50C407-7AFF-4130-A105-CC636A921B6A}">
   <dimension ref="B1:AG84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="R85" sqref="R85"/>
+    <sheetView tabSelected="1" topLeftCell="F37" workbookViewId="0">
+      <selection activeCell="AB45" sqref="AB45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -5553,11 +5553,11 @@
         <v>57</v>
       </c>
       <c r="Y44" s="16"/>
-      <c r="Z44" s="12">
-        <v>0</v>
-      </c>
-      <c r="AA44" s="16" t="s">
+      <c r="Z44" s="16" t="s">
         <v>27</v>
+      </c>
+      <c r="AA44" s="12">
+        <v>0</v>
       </c>
       <c r="AB44" s="16" t="s">
         <v>58</v>

</xml_diff>